<commit_message>
9.2 00:18 박성준 Merge
- 설정창 구현
- 비율 변경에 따른 UI 위치 조정, 카메라 콜라이더 크기 조정
- 맵 디자인 11차 적용 및 리비 이미지 적용
- 엑셀 파일 적용 및 완성물 감정 표현 적용
- 아이스 계곡 카메라 크기 조정
- 기타 연출 조정

QA29 자동으로 진행되는 스크립트에도 NPC 확대 기능 구현
QA31 이 버전부터 이전 서브섹터를 클리어하지 않으면 다음 서브섹터로 넘어갈 수 없음.
QA43 장애물 파괴 시 투명도를 천천히 낮춰서 없애는 구현
</commit_message>
<xml_diff>
--- a/Assets/Dialogs/DialogDB_Ice.xlsx
+++ b/Assets/Dialogs/DialogDB_Ice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b4d1236af1f427cd/Documents/GitHub/LGHNH_Project/Assets/Dialogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\230831_2146\LGHNH_Project\Assets\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{6153EA0C-98FF-46F8-87F9-13DD21039917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C355731-9978-4E84-A9F4-699D8C6AC03F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE7960-4CEB-47F3-A922-A2CED7030235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="10350" windowWidth="24240" windowHeight="13020" xr2:uid="{300A2B27-8A99-4D26-8917-5CDAC0CFA9B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{300A2B27-8A99-4D26-8917-5CDAC0CFA9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="ice" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="94">
   <si>
     <t>봐! 햇살이 조금씩 보이기 시작하고 있어. 어서 올라가서 몸을 녹이자. 그런 다음 모험의 종지부를 찍는거야.</t>
   </si>
@@ -56,9 +56,6 @@
     <t>준비는 됐어 리비?</t>
   </si>
   <si>
-    <t xml:space="preserve">얏호! 이제 정말 정상이 코앞이야. </t>
-  </si>
-  <si>
     <t>완료</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>앗! 저기 좀 봐! 엄청 거대한 플라고스트야!</t>
   </si>
   <si>
-    <t xml:space="preserve">이건...! 아이스카밍 민트야! </t>
-  </si>
-  <si>
     <t>다행이야. 그런데 이곳에 피어난 꽃들은 뭐지?</t>
   </si>
   <si>
@@ -315,6 +309,16 @@
   </si>
   <si>
     <t>좋아. 정상을 향해서 조금만 더 힘내보는거야!</t>
+  </si>
+  <si>
+    <t>이건...! 아이스카밍 민트야!</t>
+  </si>
+  <si>
+    <t>얏호! 이제 정말 정상이 코앞이야.</t>
+  </si>
+  <si>
+    <t>완성물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -360,16 +364,6 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="&quot;Malgun Gothic&quot;"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -380,23 +374,29 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Docs-Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -416,8 +416,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -445,11 +457,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -464,30 +506,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,17 +529,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,7 +879,7 @@
   <dimension ref="A1:H1036"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.25" defaultRowHeight="15" customHeight="1"/>
@@ -845,1416 +896,1416 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="35.25" customHeight="1" thickBot="1">
-      <c r="A1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="F1" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>74</v>
+      <c r="B2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="4">
+        <v>82</v>
+      </c>
+      <c r="E2" s="13">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="4">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="15">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="4">
+      <c r="E4" s="15">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="E5" s="15">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4">
+      <c r="E6" s="15">
         <v>1</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4">
+      <c r="E7" s="15">
         <v>1</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H7" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4">
+      <c r="E8" s="15">
         <v>1</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H8" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4">
+        <v>6</v>
+      </c>
+      <c r="E10" s="15">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="19.5" customHeight="1">
+      <c r="F10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="4">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="15">
         <v>2</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4">
+      <c r="E12" s="15">
         <v>2</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4">
+      <c r="E13" s="15">
         <v>2</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4">
+      <c r="E14" s="15">
         <v>2</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4">
+      <c r="E15" s="15">
         <v>2</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4">
+      <c r="E16" s="15">
         <v>2</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4">
+      <c r="E17" s="15">
         <v>2</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4">
+      <c r="E18" s="15">
         <v>2</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19.5" customHeight="1">
+      <c r="F18" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4">
+      <c r="E19" s="15">
         <v>2</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="19.5" customHeight="1">
+      <c r="F19" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4">
+      <c r="E20" s="15">
         <v>2</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4">
+      <c r="E21" s="15">
         <v>2</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H21" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="16" t="s">
-        <v>53</v>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="4">
+        <v>82</v>
+      </c>
+      <c r="E22" s="15">
         <v>3</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="4">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="15">
         <v>3</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="4">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="15">
         <v>3</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4">
+      <c r="E25" s="15">
         <v>3</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4">
+      <c r="E26" s="15">
         <v>3</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="4">
+      <c r="E27" s="15">
         <v>3</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4">
+      <c r="E28" s="15">
         <v>3</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H28" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4">
+      <c r="E29" s="15">
         <v>3</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4">
+      <c r="E30" s="15">
         <v>3</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H30" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H30" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="4">
+        <v>85</v>
+      </c>
+      <c r="E31" s="15">
         <v>4</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H31" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4">
+      <c r="E32" s="15">
         <v>4</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H32" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="4">
+      <c r="E33" s="15">
         <v>4</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H33" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="16" t="s">
-        <v>40</v>
+      <c r="B34" s="10"/>
+      <c r="C34" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="4">
+        <v>82</v>
+      </c>
+      <c r="E34" s="15">
         <v>5</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4">
+      <c r="E35" s="15">
         <v>5</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H35" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H35" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4">
+      <c r="E36" s="15">
         <v>5</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H36" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4">
+      <c r="E37" s="15">
         <v>5</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H37" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H37" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="4">
+      <c r="E38" s="15">
         <v>5</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G38" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="4">
+      <c r="E39" s="15">
         <v>5</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="4">
+      <c r="E40" s="15">
         <v>5</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G40" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="4">
+      <c r="E41" s="15">
         <v>5</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G41" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="4">
+      <c r="E42" s="15">
         <v>5</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G42" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="4">
+        <v>85</v>
+      </c>
+      <c r="E43" s="15">
         <v>6</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H43" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="19.5" customHeight="1">
+      <c r="H43" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="4">
+      <c r="E44" s="15">
         <v>6</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="19.5" customHeight="1">
+      <c r="G44" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="4">
+      <c r="E45" s="15">
         <v>6</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G45" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="4">
+      <c r="E46" s="15">
         <v>6</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G46" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="16" t="s">
-        <v>26</v>
+      <c r="B47" s="10"/>
+      <c r="C47" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" s="5">
+        <v>82</v>
+      </c>
+      <c r="E47" s="15">
         <v>7</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G47" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="5">
+      <c r="E48" s="15">
         <v>7</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G48" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G48" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="5">
+      <c r="E49" s="15">
         <v>7</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G49" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="5">
+      <c r="E50" s="15">
         <v>7</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G50" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G50" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="5">
+      <c r="E51" s="15">
         <v>7</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G51" s="17" t="s">
+      <c r="G51" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H51" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H51" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
       <c r="D52" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52" s="5">
+        <v>85</v>
+      </c>
+      <c r="E52" s="15">
         <v>8</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="17" t="s">
+      <c r="G52" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H52" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H52" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="5">
+      <c r="E53" s="15">
         <v>8</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="G53" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H53" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H53" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="5">
+      <c r="E54" s="15">
         <v>8</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="G54" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H54" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H54" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="5">
+      <c r="E55" s="15">
         <v>8</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G55" s="17" t="s">
+      <c r="G55" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H55" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H55" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="16" t="s">
-        <v>16</v>
+      <c r="B56" s="10"/>
+      <c r="C56" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="5">
+        <v>82</v>
+      </c>
+      <c r="E56" s="15">
         <v>9</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G56" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G56" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="5">
+      <c r="E57" s="15">
         <v>9</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G57" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G57" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="5">
+      <c r="E58" s="15">
         <v>9</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="18" t="s">
+      <c r="G58" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H58" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="5">
+      <c r="E59" s="15">
         <v>9</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G59" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G59" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="5">
+      <c r="E60" s="15">
         <v>9</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F60" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G60" s="17" t="s">
+      <c r="G60" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H60" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H60" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="5">
+      <c r="E61" s="15">
         <v>9</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G61" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H61" s="18" t="s">
+      <c r="G61" s="20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H61" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A62" s="4">
         <v>61</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
       <c r="D62" s="3"/>
-      <c r="E62" s="5">
+      <c r="E62" s="15">
         <v>9</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="G62" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H62" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H62" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
       <c r="D63" s="3"/>
-      <c r="E63" s="5">
+      <c r="E63" s="15">
         <v>9</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G63" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="16.5" customHeight="1">
+      <c r="G63" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A64" s="4">
         <v>63</v>
       </c>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="5">
+      <c r="E64" s="15">
         <v>9</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G64" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H64" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H64" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A65" s="4">
         <v>64</v>
       </c>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="5">
+      <c r="E65" s="15">
         <v>9</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="G65" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H65" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H65" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A66" s="4">
         <v>65</v>
       </c>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
       <c r="D66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E66" s="5">
+        <v>85</v>
+      </c>
+      <c r="E66" s="15">
         <v>10</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G66" s="17" t="s">
+      <c r="G66" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H66" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="16.5" customHeight="1">
+      <c r="H66" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A67" s="4">
         <v>66</v>
       </c>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="3"/>
-      <c r="E67" s="5">
+      <c r="E67" s="15">
         <v>10</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="G67" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H67" s="18" t="s">
+      <c r="H67" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="16.5" customHeight="1">
+    <row r="68" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A68" s="4">
         <v>67</v>
       </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
       <c r="D68" s="3"/>
-      <c r="E68" s="5">
+      <c r="E68" s="15">
         <v>10</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G68" s="17" t="s">
+      <c r="G68" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H68" s="18" t="s">
+      <c r="H68" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="16.5" customHeight="1">
+    <row r="69" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
       <c r="D69" s="3"/>
-      <c r="E69" s="5">
+      <c r="E69" s="15">
         <v>10</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="F69" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G69" s="17" t="s">
+      <c r="G69" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H69" s="18" t="s">
+      <c r="H69" s="21" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>